<commit_message>
Agregada la grafica de calificaciones
</commit_message>
<xml_diff>
--- a/CSOF5101 Ingeniera de Software/TSP/Util.xlsx
+++ b/CSOF5101 Ingeniera de Software/TSP/Util.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="180">
   <si>
     <t>b0</t>
   </si>
@@ -489,16 +489,73 @@
     <t xml:space="preserve"> @LogT(cycle = CYCLE_2, date = "</t>
   </si>
   <si>
-    <t>David Pérez</t>
-  </si>
-  <si>
     <t>sandra</t>
   </si>
   <si>
     <t>carlos</t>
   </si>
   <si>
-    <t>erik</t>
+    <t>1.5.6.1</t>
+  </si>
+  <si>
+    <t>1.5.6.2</t>
+  </si>
+  <si>
+    <t>1.5.1.1</t>
+  </si>
+  <si>
+    <t>1.5.1.2</t>
+  </si>
+  <si>
+    <t>1.5.1.4</t>
+  </si>
+  <si>
+    <t>1.5.2.3</t>
+  </si>
+  <si>
+    <t>1.5.3.2</t>
+  </si>
+  <si>
+    <t>1.5.4.2</t>
+  </si>
+  <si>
+    <t>1.5.5.6</t>
+  </si>
+  <si>
+    <t>1.5.5.7</t>
+  </si>
+  <si>
+    <t>1.5.5.1</t>
+  </si>
+  <si>
+    <t>1.5.5.2</t>
+  </si>
+  <si>
+    <t>1.5.7.3</t>
+  </si>
+  <si>
+    <t>1.5.1.3</t>
+  </si>
+  <si>
+    <t>1.5.2.1</t>
+  </si>
+  <si>
+    <t>1.5.5.3</t>
+  </si>
+  <si>
+    <t>1.5.5.5</t>
+  </si>
+  <si>
+    <t>1.5.6.3</t>
+  </si>
+  <si>
+    <t>1.5.7.1</t>
+  </si>
+  <si>
+    <t>1.5.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @LogT(cycle = CYCLE_3, date = "</t>
   </si>
 </sst>
 </file>
@@ -886,11 +943,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="46553728"/>
-        <c:axId val="46576768"/>
+        <c:axId val="68598400"/>
+        <c:axId val="68760704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46553728"/>
+        <c:axId val="68598400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -932,13 +989,13 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46576768"/>
+        <c:crossAx val="68760704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46576768"/>
+        <c:axId val="68760704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -980,7 +1037,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46553728"/>
+        <c:crossAx val="68598400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1011,7 +1068,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1093,19 +1150,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
@@ -1164,13 +1221,13 @@
                   <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
@@ -1232,16 +1289,16 @@
                   <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
@@ -1297,19 +1354,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.2</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.8</c:v>
@@ -1318,11 +1375,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="46595456"/>
-        <c:axId val="77633024"/>
+        <c:axId val="68808064"/>
+        <c:axId val="68920832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46595456"/>
+        <c:axId val="68808064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,14 +1404,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77633024"/>
+        <c:crossAx val="68920832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77633024"/>
+        <c:axId val="68920832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1382,7 +1439,7 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46595456"/>
+        <c:crossAx val="68808064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1400,7 +1457,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2111,11 +2168,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:AA187"/>
+  <dimension ref="B2:AA238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D36" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46:N50"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
@@ -2458,13 +2513,13 @@
     </row>
     <row r="36" spans="3:27">
       <c r="C36" t="s">
-        <v>157</v>
+        <v>17</v>
       </c>
       <c r="D36" s="12">
         <v>5</v>
       </c>
       <c r="E36" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F36" s="11">
         <v>5</v>
@@ -2473,25 +2528,25 @@
         <v>4</v>
       </c>
       <c r="H36" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I36" s="11">
         <v>5</v>
       </c>
       <c r="J36" s="11">
+        <v>5</v>
+      </c>
+      <c r="K36" s="10">
+        <v>5</v>
+      </c>
+      <c r="L36" s="12">
+        <v>5</v>
+      </c>
+      <c r="M36" s="11">
+        <v>5</v>
+      </c>
+      <c r="N36" s="11">
         <v>4</v>
-      </c>
-      <c r="K36" s="10">
-        <v>4</v>
-      </c>
-      <c r="L36" s="12">
-        <v>5</v>
-      </c>
-      <c r="M36" s="11">
-        <v>5</v>
-      </c>
-      <c r="N36" s="11">
-        <v>5</v>
       </c>
       <c r="O36" s="10">
         <v>4</v>
@@ -2510,7 +2565,7 @@
         <v>5</v>
       </c>
       <c r="W36" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X36" s="12">
         <v>5</v>
@@ -2527,10 +2582,10 @@
     </row>
     <row r="37" spans="3:27">
       <c r="C37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D37" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E37" s="11">
         <v>5</v>
@@ -2545,15 +2600,23 @@
       <c r="I37" s="11"/>
       <c r="J37" s="11"/>
       <c r="K37" s="10"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="10"/>
+      <c r="L37" s="12">
+        <v>5</v>
+      </c>
+      <c r="M37" s="11">
+        <v>4</v>
+      </c>
+      <c r="N37" s="11">
+        <v>5</v>
+      </c>
+      <c r="O37" s="10">
+        <v>5</v>
+      </c>
       <c r="P37" s="12">
         <v>4</v>
       </c>
       <c r="Q37" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R37" s="11">
         <v>5</v>
@@ -2588,19 +2651,19 @@
     </row>
     <row r="38" spans="3:27">
       <c r="C38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D38" s="12">
         <v>4</v>
       </c>
       <c r="E38" s="11">
+        <v>5</v>
+      </c>
+      <c r="F38" s="11">
         <v>4</v>
       </c>
-      <c r="F38" s="11">
-        <v>5</v>
-      </c>
       <c r="G38" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H38" s="12">
         <v>4</v>
@@ -2609,10 +2672,10 @@
         <v>5</v>
       </c>
       <c r="J38" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K38" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L38" s="12">
         <v>4</v>
@@ -2621,16 +2684,16 @@
         <v>5</v>
       </c>
       <c r="N38" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O38" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P38" s="12">
         <v>4</v>
       </c>
       <c r="Q38" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R38" s="11">
         <v>4</v>
@@ -2638,26 +2701,26 @@
       <c r="S38" s="10">
         <v>4</v>
       </c>
-      <c r="T38" s="12"/>
-      <c r="U38" s="11"/>
-      <c r="V38" s="11"/>
-      <c r="W38" s="10"/>
-      <c r="X38" s="12">
-        <v>5</v>
-      </c>
-      <c r="Y38" s="11">
-        <v>5</v>
-      </c>
-      <c r="Z38" s="11">
-        <v>5</v>
-      </c>
-      <c r="AA38" s="10">
-        <v>5</v>
-      </c>
+      <c r="T38" s="12">
+        <v>4</v>
+      </c>
+      <c r="U38" s="11">
+        <v>5</v>
+      </c>
+      <c r="V38" s="11">
+        <v>5</v>
+      </c>
+      <c r="W38" s="10">
+        <v>4</v>
+      </c>
+      <c r="X38" s="12"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="11"/>
+      <c r="AA38" s="10"/>
     </row>
     <row r="39" spans="3:27">
       <c r="C39" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D39" s="12">
         <v>4</v>
@@ -2669,7 +2732,7 @@
         <v>5</v>
       </c>
       <c r="G39" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H39" s="12">
         <v>4</v>
@@ -2681,36 +2744,36 @@
         <v>5</v>
       </c>
       <c r="K39" s="10">
-        <v>5</v>
-      </c>
-      <c r="L39" s="12"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="L39" s="12">
+        <v>4</v>
+      </c>
+      <c r="M39" s="11">
+        <v>5</v>
+      </c>
+      <c r="N39" s="11">
+        <v>5</v>
+      </c>
+      <c r="O39" s="10">
+        <v>5</v>
+      </c>
       <c r="P39" s="12">
         <v>4</v>
       </c>
       <c r="Q39" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R39" s="11">
         <v>5</v>
       </c>
       <c r="S39" s="10">
-        <v>4</v>
-      </c>
-      <c r="T39" s="12">
-        <v>5</v>
-      </c>
-      <c r="U39" s="11">
-        <v>5</v>
-      </c>
-      <c r="V39" s="11">
-        <v>5</v>
-      </c>
-      <c r="W39" s="10">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="T39" s="12"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="10"/>
       <c r="X39" s="12">
         <v>5</v>
       </c>
@@ -2726,23 +2789,23 @@
     </row>
     <row r="40" spans="3:27">
       <c r="C40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="10"/>
       <c r="H40" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I40" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J40" s="11">
         <v>5</v>
       </c>
       <c r="K40" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L40" s="12">
         <v>5</v>
@@ -2751,13 +2814,13 @@
         <v>5</v>
       </c>
       <c r="N40" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O40" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P40" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q40" s="11">
         <v>5</v>
@@ -2766,7 +2829,7 @@
         <v>5</v>
       </c>
       <c r="S40" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T40" s="12">
         <v>5</v>
@@ -2775,7 +2838,7 @@
         <v>5</v>
       </c>
       <c r="V40" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W40" s="10">
         <v>5</v>
@@ -2795,7 +2858,7 @@
     </row>
     <row r="41" spans="3:27">
       <c r="C41" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D41" s="9">
         <v>5</v>
@@ -2804,35 +2867,27 @@
         <v>5</v>
       </c>
       <c r="F41" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G41" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H41" s="9">
         <v>4</v>
       </c>
       <c r="I41" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J41" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K41" s="7">
-        <v>4</v>
-      </c>
-      <c r="L41" s="9">
-        <v>4</v>
-      </c>
-      <c r="M41" s="8">
-        <v>5</v>
-      </c>
-      <c r="N41" s="8">
-        <v>5</v>
-      </c>
-      <c r="O41" s="7">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="L41" s="9"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="7"/>
       <c r="P41" s="9">
         <v>4</v>
       </c>
@@ -2840,10 +2895,10 @@
         <v>5</v>
       </c>
       <c r="R41" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S41" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T41" s="9">
         <v>5</v>
@@ -2852,15 +2907,23 @@
         <v>5</v>
       </c>
       <c r="V41" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W41" s="7">
         <v>5</v>
       </c>
-      <c r="X41" s="9"/>
-      <c r="Y41" s="8"/>
-      <c r="Z41" s="8"/>
-      <c r="AA41" s="7"/>
+      <c r="X41" s="9">
+        <v>5</v>
+      </c>
+      <c r="Y41" s="8">
+        <v>5</v>
+      </c>
+      <c r="Z41" s="8">
+        <v>5</v>
+      </c>
+      <c r="AA41" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="45" spans="3:27">
       <c r="H45" t="s">
@@ -2888,7 +2951,7 @@
       </c>
       <c r="H46" s="6">
         <f>ROUND(AVERAGE(D36:D41),2)</f>
-        <v>4.5999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I46" s="6">
         <f>ROUND(AVERAGE(H36:H41),2)</f>
@@ -2896,15 +2959,15 @@
       </c>
       <c r="J46" s="6">
         <f>ROUND(AVERAGE(L36:L41),2)</f>
-        <v>4.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="K46" s="6">
         <f>ROUND(AVERAGE(P36:P41),2)</f>
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="L46" s="6">
         <f>ROUND(AVERAGE(T36:T41),2)</f>
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="M46" s="6">
         <f>ROUND(AVERAGE(X36:X41),2)</f>
@@ -2912,7 +2975,7 @@
       </c>
       <c r="N46" s="6">
         <f>AVERAGE(H46:M46)</f>
-        <v>4.55</v>
+        <v>4.5333333333333341</v>
       </c>
     </row>
     <row r="47" spans="3:27">
@@ -2925,15 +2988,15 @@
       </c>
       <c r="I47" s="6">
         <f>ROUND(AVERAGE(I36:I41),2)</f>
-        <v>4.5999999999999996</v>
+        <v>5</v>
       </c>
       <c r="J47" s="6">
         <f>ROUND(AVERAGE(M36:M41),2)</f>
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="K47" s="6">
         <f>ROUND(AVERAGE(Q36:Q41),2)</f>
-        <v>4.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="L47" s="6">
         <f>ROUND(AVERAGE(U36:U41),2)</f>
@@ -2945,7 +3008,7 @@
       </c>
       <c r="N47" s="6">
         <f>AVERAGE(H47:M47)</f>
-        <v>4.8666666666666663</v>
+        <v>4.8666666666666671</v>
       </c>
     </row>
     <row r="48" spans="3:27">
@@ -2958,19 +3021,19 @@
       </c>
       <c r="I48" s="6">
         <f>ROUND(AVERAGE(J36:J41),2)</f>
-        <v>4.5999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="J48" s="6">
         <f>ROUND(AVERAGE(N36:N41),2)</f>
-        <v>4.5</v>
+        <v>4.8</v>
       </c>
       <c r="K48" s="6">
         <f>ROUND(AVERAGE(R36:R41),2)</f>
-        <v>4.5999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="L48" s="6">
         <f>ROUND(AVERAGE(V36:V41),2)</f>
-        <v>4.5999999999999996</v>
+        <v>5</v>
       </c>
       <c r="M48" s="6">
         <f>ROUND(AVERAGE(Z36:Z41),2)</f>
@@ -2978,7 +3041,7 @@
       </c>
       <c r="N48" s="6">
         <f>AVERAGE(H48:M48)</f>
-        <v>4.6833333333333336</v>
+        <v>4.8666666666666663</v>
       </c>
     </row>
     <row r="49" spans="7:14">
@@ -2987,23 +3050,23 @@
       </c>
       <c r="H49" s="6">
         <f>ROUND(AVERAGE(G36:G41),2)</f>
-        <v>4.4000000000000004</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I49" s="6">
         <f>ROUND(AVERAGE(K36:K41),2)</f>
-        <v>4.2</v>
+        <v>4.8</v>
       </c>
       <c r="J49" s="6">
         <f>ROUND(AVERAGE(O36:O41),2)</f>
-        <v>4</v>
+        <v>4.8</v>
       </c>
       <c r="K49" s="6">
         <f>ROUND(AVERAGE(S36:S41),2)</f>
-        <v>4.2</v>
+        <v>4.8</v>
       </c>
       <c r="L49" s="6">
         <f>ROUND(AVERAGE(W36:W41),2)</f>
-        <v>4.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="M49" s="6">
         <f>ROUND(AVERAGE(AA36:AA41),2)</f>
@@ -3011,7 +3074,7 @@
       </c>
       <c r="N49" s="6">
         <f>AVERAGE(H49:M49)</f>
-        <v>4.4000000000000004</v>
+        <v>4.7333333333333334</v>
       </c>
     </row>
     <row r="50" spans="7:14">
@@ -3021,15 +3084,15 @@
       </c>
       <c r="I50" s="6">
         <f t="shared" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
       <c r="J50" s="6">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="K50" s="6">
         <f t="shared" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>4.6000000000000005</v>
       </c>
       <c r="L50" s="6">
         <f t="shared" si="1"/>
@@ -5736,28 +5799,28 @@
         <v>156</v>
       </c>
       <c r="E137" s="16">
-        <f t="shared" ref="E136:E187" si="10">R137</f>
+        <f t="shared" ref="E137:E187" si="10">R137</f>
         <v>40620</v>
       </c>
       <c r="F137" t="s">
         <v>50</v>
       </c>
       <c r="G137" t="str">
-        <f t="shared" ref="G136:G187" si="11">Q137</f>
+        <f t="shared" ref="G137:G187" si="11">Q137</f>
         <v>1.4.1.1</v>
       </c>
       <c r="H137" t="s">
         <v>49</v>
       </c>
       <c r="I137">
-        <f t="shared" ref="I136:I187" si="12">P137</f>
+        <f t="shared" ref="I137:I187" si="12">P137</f>
         <v>201110544</v>
       </c>
       <c r="J137" t="s">
         <v>48</v>
       </c>
       <c r="K137">
-        <f t="shared" ref="K136:K187" si="13">S137</f>
+        <f t="shared" ref="K137:K187" si="13">S137</f>
         <v>60</v>
       </c>
       <c r="L137" t="s">
@@ -8024,6 +8087,2259 @@
       </c>
       <c r="S187">
         <v>120</v>
+      </c>
+    </row>
+    <row r="188" spans="4:19">
+      <c r="E188" s="16"/>
+    </row>
+    <row r="189" spans="4:19">
+      <c r="D189" t="s">
+        <v>179</v>
+      </c>
+      <c r="E189" s="16">
+        <f t="shared" ref="E188:E238" si="14">R189</f>
+        <v>40629</v>
+      </c>
+      <c r="F189" t="s">
+        <v>50</v>
+      </c>
+      <c r="G189" t="str">
+        <f t="shared" ref="G188:G238" si="15">Q189</f>
+        <v>1.5.6.1</v>
+      </c>
+      <c r="H189" t="s">
+        <v>49</v>
+      </c>
+      <c r="I189">
+        <f t="shared" ref="I188:I238" si="16">P189</f>
+        <v>201110544</v>
+      </c>
+      <c r="J189" t="s">
+        <v>48</v>
+      </c>
+      <c r="K189">
+        <f t="shared" ref="K188:K238" si="17">S189</f>
+        <v>120</v>
+      </c>
+      <c r="L189" t="s">
+        <v>47</v>
+      </c>
+      <c r="P189">
+        <v>201110544</v>
+      </c>
+      <c r="Q189" t="s">
+        <v>159</v>
+      </c>
+      <c r="R189" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S189">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="190" spans="4:19">
+      <c r="D190" t="s">
+        <v>179</v>
+      </c>
+      <c r="E190" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F190" t="s">
+        <v>50</v>
+      </c>
+      <c r="G190" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.6.2</v>
+      </c>
+      <c r="H190" t="s">
+        <v>49</v>
+      </c>
+      <c r="I190">
+        <f t="shared" si="16"/>
+        <v>201110544</v>
+      </c>
+      <c r="J190" t="s">
+        <v>48</v>
+      </c>
+      <c r="K190">
+        <f t="shared" si="17"/>
+        <v>60</v>
+      </c>
+      <c r="L190" t="s">
+        <v>47</v>
+      </c>
+      <c r="P190">
+        <v>201110544</v>
+      </c>
+      <c r="Q190" t="s">
+        <v>160</v>
+      </c>
+      <c r="R190" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S190">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="191" spans="4:19">
+      <c r="D191" t="s">
+        <v>179</v>
+      </c>
+      <c r="E191" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F191" t="s">
+        <v>50</v>
+      </c>
+      <c r="G191" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.1.1</v>
+      </c>
+      <c r="H191" t="s">
+        <v>49</v>
+      </c>
+      <c r="I191">
+        <f t="shared" si="16"/>
+        <v>201110949</v>
+      </c>
+      <c r="J191" t="s">
+        <v>48</v>
+      </c>
+      <c r="K191">
+        <f t="shared" si="17"/>
+        <v>60</v>
+      </c>
+      <c r="L191" t="s">
+        <v>47</v>
+      </c>
+      <c r="P191">
+        <v>201110949</v>
+      </c>
+      <c r="Q191" t="s">
+        <v>161</v>
+      </c>
+      <c r="R191" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S191">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="192" spans="4:19">
+      <c r="D192" t="s">
+        <v>179</v>
+      </c>
+      <c r="E192" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F192" t="s">
+        <v>50</v>
+      </c>
+      <c r="G192" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.1.2</v>
+      </c>
+      <c r="H192" t="s">
+        <v>49</v>
+      </c>
+      <c r="I192">
+        <f t="shared" si="16"/>
+        <v>201110949</v>
+      </c>
+      <c r="J192" t="s">
+        <v>48</v>
+      </c>
+      <c r="K192">
+        <f t="shared" si="17"/>
+        <v>30</v>
+      </c>
+      <c r="L192" t="s">
+        <v>47</v>
+      </c>
+      <c r="P192">
+        <v>201110949</v>
+      </c>
+      <c r="Q192" t="s">
+        <v>162</v>
+      </c>
+      <c r="R192" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S192">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="193" spans="4:19">
+      <c r="D193" t="s">
+        <v>179</v>
+      </c>
+      <c r="E193" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F193" t="s">
+        <v>50</v>
+      </c>
+      <c r="G193" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.1.4</v>
+      </c>
+      <c r="H193" t="s">
+        <v>49</v>
+      </c>
+      <c r="I193">
+        <f t="shared" si="16"/>
+        <v>201110949</v>
+      </c>
+      <c r="J193" t="s">
+        <v>48</v>
+      </c>
+      <c r="K193">
+        <f t="shared" si="17"/>
+        <v>20</v>
+      </c>
+      <c r="L193" t="s">
+        <v>47</v>
+      </c>
+      <c r="P193">
+        <v>201110949</v>
+      </c>
+      <c r="Q193" t="s">
+        <v>163</v>
+      </c>
+      <c r="R193" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S193">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="194" spans="4:19">
+      <c r="D194" t="s">
+        <v>179</v>
+      </c>
+      <c r="E194" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F194" t="s">
+        <v>50</v>
+      </c>
+      <c r="G194" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.2.3</v>
+      </c>
+      <c r="H194" t="s">
+        <v>49</v>
+      </c>
+      <c r="I194">
+        <f t="shared" si="16"/>
+        <v>201110949</v>
+      </c>
+      <c r="J194" t="s">
+        <v>48</v>
+      </c>
+      <c r="K194">
+        <f t="shared" si="17"/>
+        <v>30</v>
+      </c>
+      <c r="L194" t="s">
+        <v>47</v>
+      </c>
+      <c r="P194">
+        <v>201110949</v>
+      </c>
+      <c r="Q194" t="s">
+        <v>164</v>
+      </c>
+      <c r="R194" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S194">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="195" spans="4:19">
+      <c r="D195" t="s">
+        <v>179</v>
+      </c>
+      <c r="E195" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F195" t="s">
+        <v>50</v>
+      </c>
+      <c r="G195" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.3.2</v>
+      </c>
+      <c r="H195" t="s">
+        <v>49</v>
+      </c>
+      <c r="I195">
+        <f t="shared" si="16"/>
+        <v>201110949</v>
+      </c>
+      <c r="J195" t="s">
+        <v>48</v>
+      </c>
+      <c r="K195">
+        <f t="shared" si="17"/>
+        <v>15</v>
+      </c>
+      <c r="L195" t="s">
+        <v>47</v>
+      </c>
+      <c r="P195">
+        <v>201110949</v>
+      </c>
+      <c r="Q195" t="s">
+        <v>165</v>
+      </c>
+      <c r="R195" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S195">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="196" spans="4:19">
+      <c r="D196" t="s">
+        <v>179</v>
+      </c>
+      <c r="E196" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F196" t="s">
+        <v>50</v>
+      </c>
+      <c r="G196" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.4.2</v>
+      </c>
+      <c r="H196" t="s">
+        <v>49</v>
+      </c>
+      <c r="I196">
+        <f t="shared" si="16"/>
+        <v>201110949</v>
+      </c>
+      <c r="J196" t="s">
+        <v>48</v>
+      </c>
+      <c r="K196">
+        <f t="shared" si="17"/>
+        <v>15</v>
+      </c>
+      <c r="L196" t="s">
+        <v>47</v>
+      </c>
+      <c r="P196">
+        <v>201110949</v>
+      </c>
+      <c r="Q196" t="s">
+        <v>166</v>
+      </c>
+      <c r="R196" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S196">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="197" spans="4:19">
+      <c r="D197" t="s">
+        <v>179</v>
+      </c>
+      <c r="E197" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F197" t="s">
+        <v>50</v>
+      </c>
+      <c r="G197" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.6</v>
+      </c>
+      <c r="H197" t="s">
+        <v>49</v>
+      </c>
+      <c r="I197">
+        <f t="shared" si="16"/>
+        <v>201110949</v>
+      </c>
+      <c r="J197" t="s">
+        <v>48</v>
+      </c>
+      <c r="K197">
+        <f t="shared" si="17"/>
+        <v>80</v>
+      </c>
+      <c r="L197" t="s">
+        <v>47</v>
+      </c>
+      <c r="P197">
+        <v>201110949</v>
+      </c>
+      <c r="Q197" t="s">
+        <v>167</v>
+      </c>
+      <c r="R197" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S197">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="198" spans="4:19">
+      <c r="D198" t="s">
+        <v>179</v>
+      </c>
+      <c r="E198" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F198" t="s">
+        <v>50</v>
+      </c>
+      <c r="G198" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.7</v>
+      </c>
+      <c r="H198" t="s">
+        <v>49</v>
+      </c>
+      <c r="I198">
+        <f t="shared" si="16"/>
+        <v>201110949</v>
+      </c>
+      <c r="J198" t="s">
+        <v>48</v>
+      </c>
+      <c r="K198">
+        <f t="shared" si="17"/>
+        <v>30</v>
+      </c>
+      <c r="L198" t="s">
+        <v>47</v>
+      </c>
+      <c r="P198">
+        <v>201110949</v>
+      </c>
+      <c r="Q198" t="s">
+        <v>168</v>
+      </c>
+      <c r="R198" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S198">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="199" spans="4:19">
+      <c r="D199" t="s">
+        <v>179</v>
+      </c>
+      <c r="E199" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F199" t="s">
+        <v>50</v>
+      </c>
+      <c r="G199" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.1</v>
+      </c>
+      <c r="H199" t="s">
+        <v>49</v>
+      </c>
+      <c r="I199">
+        <f t="shared" si="16"/>
+        <v>201110949</v>
+      </c>
+      <c r="J199" t="s">
+        <v>48</v>
+      </c>
+      <c r="K199">
+        <f t="shared" si="17"/>
+        <v>30</v>
+      </c>
+      <c r="L199" t="s">
+        <v>47</v>
+      </c>
+      <c r="P199">
+        <v>201110949</v>
+      </c>
+      <c r="Q199" t="s">
+        <v>169</v>
+      </c>
+      <c r="R199" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S199">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="200" spans="4:19">
+      <c r="D200" t="s">
+        <v>179</v>
+      </c>
+      <c r="E200" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F200" t="s">
+        <v>50</v>
+      </c>
+      <c r="G200" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.2</v>
+      </c>
+      <c r="H200" t="s">
+        <v>49</v>
+      </c>
+      <c r="I200">
+        <f t="shared" si="16"/>
+        <v>201110949</v>
+      </c>
+      <c r="J200" t="s">
+        <v>48</v>
+      </c>
+      <c r="K200">
+        <f t="shared" si="17"/>
+        <v>30</v>
+      </c>
+      <c r="L200" t="s">
+        <v>47</v>
+      </c>
+      <c r="P200">
+        <v>201110949</v>
+      </c>
+      <c r="Q200" t="s">
+        <v>170</v>
+      </c>
+      <c r="R200" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S200">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="201" spans="4:19">
+      <c r="D201" t="s">
+        <v>179</v>
+      </c>
+      <c r="E201" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F201" t="s">
+        <v>50</v>
+      </c>
+      <c r="G201" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.7.3</v>
+      </c>
+      <c r="H201" t="s">
+        <v>49</v>
+      </c>
+      <c r="I201">
+        <f t="shared" si="16"/>
+        <v>201110949</v>
+      </c>
+      <c r="J201" t="s">
+        <v>48</v>
+      </c>
+      <c r="K201">
+        <f t="shared" si="17"/>
+        <v>15</v>
+      </c>
+      <c r="L201" t="s">
+        <v>47</v>
+      </c>
+      <c r="P201">
+        <v>201110949</v>
+      </c>
+      <c r="Q201" t="s">
+        <v>171</v>
+      </c>
+      <c r="R201" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S201">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="202" spans="4:19">
+      <c r="D202" t="s">
+        <v>179</v>
+      </c>
+      <c r="E202" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F202" t="s">
+        <v>50</v>
+      </c>
+      <c r="G202" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.1.1</v>
+      </c>
+      <c r="H202" t="s">
+        <v>49</v>
+      </c>
+      <c r="I202">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J202" t="s">
+        <v>48</v>
+      </c>
+      <c r="K202">
+        <f t="shared" si="17"/>
+        <v>40</v>
+      </c>
+      <c r="L202" t="s">
+        <v>47</v>
+      </c>
+      <c r="P202">
+        <v>201110951</v>
+      </c>
+      <c r="Q202" t="s">
+        <v>161</v>
+      </c>
+      <c r="R202" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S202">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="203" spans="4:19">
+      <c r="D203" t="s">
+        <v>179</v>
+      </c>
+      <c r="E203" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F203" t="s">
+        <v>50</v>
+      </c>
+      <c r="G203" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.1.3</v>
+      </c>
+      <c r="H203" t="s">
+        <v>49</v>
+      </c>
+      <c r="I203">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J203" t="s">
+        <v>48</v>
+      </c>
+      <c r="K203">
+        <f t="shared" si="17"/>
+        <v>20</v>
+      </c>
+      <c r="L203" t="s">
+        <v>47</v>
+      </c>
+      <c r="P203">
+        <v>201110951</v>
+      </c>
+      <c r="Q203" t="s">
+        <v>172</v>
+      </c>
+      <c r="R203" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S203">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="204" spans="4:19">
+      <c r="D204" t="s">
+        <v>179</v>
+      </c>
+      <c r="E204" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F204" t="s">
+        <v>50</v>
+      </c>
+      <c r="G204" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.1.4</v>
+      </c>
+      <c r="H204" t="s">
+        <v>49</v>
+      </c>
+      <c r="I204">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J204" t="s">
+        <v>48</v>
+      </c>
+      <c r="K204">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="L204" t="s">
+        <v>47</v>
+      </c>
+      <c r="P204">
+        <v>201110951</v>
+      </c>
+      <c r="Q204" t="s">
+        <v>163</v>
+      </c>
+      <c r="R204" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S204">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="205" spans="4:19">
+      <c r="D205" t="s">
+        <v>179</v>
+      </c>
+      <c r="E205" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F205" t="s">
+        <v>50</v>
+      </c>
+      <c r="G205" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.2.1</v>
+      </c>
+      <c r="H205" t="s">
+        <v>49</v>
+      </c>
+      <c r="I205">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J205" t="s">
+        <v>48</v>
+      </c>
+      <c r="K205">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="L205" t="s">
+        <v>47</v>
+      </c>
+      <c r="P205">
+        <v>201110951</v>
+      </c>
+      <c r="Q205" t="s">
+        <v>173</v>
+      </c>
+      <c r="R205" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S205">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="206" spans="4:19">
+      <c r="D206" t="s">
+        <v>179</v>
+      </c>
+      <c r="E206" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F206" t="s">
+        <v>50</v>
+      </c>
+      <c r="G206" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.2.3</v>
+      </c>
+      <c r="H206" t="s">
+        <v>49</v>
+      </c>
+      <c r="I206">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J206" t="s">
+        <v>48</v>
+      </c>
+      <c r="K206">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="L206" t="s">
+        <v>47</v>
+      </c>
+      <c r="P206">
+        <v>201110951</v>
+      </c>
+      <c r="Q206" t="s">
+        <v>164</v>
+      </c>
+      <c r="R206" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S206">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207" spans="4:19">
+      <c r="D207" t="s">
+        <v>179</v>
+      </c>
+      <c r="E207" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F207" t="s">
+        <v>50</v>
+      </c>
+      <c r="G207" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.3.2</v>
+      </c>
+      <c r="H207" t="s">
+        <v>49</v>
+      </c>
+      <c r="I207">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J207" t="s">
+        <v>48</v>
+      </c>
+      <c r="K207">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="L207" t="s">
+        <v>47</v>
+      </c>
+      <c r="P207">
+        <v>201110951</v>
+      </c>
+      <c r="Q207" t="s">
+        <v>165</v>
+      </c>
+      <c r="R207" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S207">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="208" spans="4:19">
+      <c r="D208" t="s">
+        <v>179</v>
+      </c>
+      <c r="E208" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F208" t="s">
+        <v>50</v>
+      </c>
+      <c r="G208" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.4.2</v>
+      </c>
+      <c r="H208" t="s">
+        <v>49</v>
+      </c>
+      <c r="I208">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J208" t="s">
+        <v>48</v>
+      </c>
+      <c r="K208">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="L208" t="s">
+        <v>47</v>
+      </c>
+      <c r="P208">
+        <v>201110951</v>
+      </c>
+      <c r="Q208" t="s">
+        <v>166</v>
+      </c>
+      <c r="R208" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S208">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="209" spans="4:19">
+      <c r="D209" t="s">
+        <v>179</v>
+      </c>
+      <c r="E209" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F209" t="s">
+        <v>50</v>
+      </c>
+      <c r="G209" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.3</v>
+      </c>
+      <c r="H209" t="s">
+        <v>49</v>
+      </c>
+      <c r="I209">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J209" t="s">
+        <v>48</v>
+      </c>
+      <c r="K209">
+        <f t="shared" si="17"/>
+        <v>240</v>
+      </c>
+      <c r="L209" t="s">
+        <v>47</v>
+      </c>
+      <c r="P209">
+        <v>201110951</v>
+      </c>
+      <c r="Q209" t="s">
+        <v>174</v>
+      </c>
+      <c r="R209" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S209">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="210" spans="4:19">
+      <c r="D210" t="s">
+        <v>179</v>
+      </c>
+      <c r="E210" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F210" t="s">
+        <v>50</v>
+      </c>
+      <c r="G210" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.3</v>
+      </c>
+      <c r="H210" t="s">
+        <v>49</v>
+      </c>
+      <c r="I210">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J210" t="s">
+        <v>48</v>
+      </c>
+      <c r="K210">
+        <f t="shared" si="17"/>
+        <v>60</v>
+      </c>
+      <c r="L210" t="s">
+        <v>47</v>
+      </c>
+      <c r="P210">
+        <v>201110951</v>
+      </c>
+      <c r="Q210" t="s">
+        <v>174</v>
+      </c>
+      <c r="R210" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S210">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="211" spans="4:19">
+      <c r="D211" t="s">
+        <v>179</v>
+      </c>
+      <c r="E211" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F211" t="s">
+        <v>50</v>
+      </c>
+      <c r="G211" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.2</v>
+      </c>
+      <c r="H211" t="s">
+        <v>49</v>
+      </c>
+      <c r="I211">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J211" t="s">
+        <v>48</v>
+      </c>
+      <c r="K211">
+        <f t="shared" si="17"/>
+        <v>120</v>
+      </c>
+      <c r="L211" t="s">
+        <v>47</v>
+      </c>
+      <c r="P211">
+        <v>201110951</v>
+      </c>
+      <c r="Q211" t="s">
+        <v>170</v>
+      </c>
+      <c r="R211" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S211">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="212" spans="4:19">
+      <c r="D212" t="s">
+        <v>179</v>
+      </c>
+      <c r="E212" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F212" t="s">
+        <v>50</v>
+      </c>
+      <c r="G212" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.5</v>
+      </c>
+      <c r="H212" t="s">
+        <v>49</v>
+      </c>
+      <c r="I212">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J212" t="s">
+        <v>48</v>
+      </c>
+      <c r="K212">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="L212" t="s">
+        <v>47</v>
+      </c>
+      <c r="P212">
+        <v>201110951</v>
+      </c>
+      <c r="Q212" t="s">
+        <v>175</v>
+      </c>
+      <c r="R212" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S212">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="213" spans="4:19">
+      <c r="D213" t="s">
+        <v>179</v>
+      </c>
+      <c r="E213" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F213" t="s">
+        <v>50</v>
+      </c>
+      <c r="G213" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.6</v>
+      </c>
+      <c r="H213" t="s">
+        <v>49</v>
+      </c>
+      <c r="I213">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J213" t="s">
+        <v>48</v>
+      </c>
+      <c r="K213">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="L213" t="s">
+        <v>47</v>
+      </c>
+      <c r="P213">
+        <v>201110951</v>
+      </c>
+      <c r="Q213" t="s">
+        <v>167</v>
+      </c>
+      <c r="R213" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S213">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="4:19">
+      <c r="D214" t="s">
+        <v>179</v>
+      </c>
+      <c r="E214" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F214" t="s">
+        <v>50</v>
+      </c>
+      <c r="G214" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.7</v>
+      </c>
+      <c r="H214" t="s">
+        <v>49</v>
+      </c>
+      <c r="I214">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J214" t="s">
+        <v>48</v>
+      </c>
+      <c r="K214">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="L214" t="s">
+        <v>47</v>
+      </c>
+      <c r="P214">
+        <v>201110951</v>
+      </c>
+      <c r="Q214" t="s">
+        <v>168</v>
+      </c>
+      <c r="R214" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S214">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="215" spans="4:19">
+      <c r="D215" t="s">
+        <v>179</v>
+      </c>
+      <c r="E215" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F215" t="s">
+        <v>50</v>
+      </c>
+      <c r="G215" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.6.1</v>
+      </c>
+      <c r="H215" t="s">
+        <v>49</v>
+      </c>
+      <c r="I215">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J215" t="s">
+        <v>48</v>
+      </c>
+      <c r="K215">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="L215" t="s">
+        <v>47</v>
+      </c>
+      <c r="P215">
+        <v>201110951</v>
+      </c>
+      <c r="Q215" t="s">
+        <v>159</v>
+      </c>
+      <c r="R215" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S215">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="216" spans="4:19">
+      <c r="D216" t="s">
+        <v>179</v>
+      </c>
+      <c r="E216" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F216" t="s">
+        <v>50</v>
+      </c>
+      <c r="G216" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.6.3</v>
+      </c>
+      <c r="H216" t="s">
+        <v>49</v>
+      </c>
+      <c r="I216">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J216" t="s">
+        <v>48</v>
+      </c>
+      <c r="K216">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="L216" t="s">
+        <v>47</v>
+      </c>
+      <c r="P216">
+        <v>201110951</v>
+      </c>
+      <c r="Q216" t="s">
+        <v>176</v>
+      </c>
+      <c r="R216" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S216">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="217" spans="4:19">
+      <c r="D217" t="s">
+        <v>179</v>
+      </c>
+      <c r="E217" s="16">
+        <f t="shared" si="14"/>
+        <v>40630</v>
+      </c>
+      <c r="F217" t="s">
+        <v>50</v>
+      </c>
+      <c r="G217" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.7.1</v>
+      </c>
+      <c r="H217" t="s">
+        <v>49</v>
+      </c>
+      <c r="I217">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J217" t="s">
+        <v>48</v>
+      </c>
+      <c r="K217">
+        <f t="shared" si="17"/>
+        <v>90</v>
+      </c>
+      <c r="L217" t="s">
+        <v>47</v>
+      </c>
+      <c r="P217">
+        <v>201110951</v>
+      </c>
+      <c r="Q217" t="s">
+        <v>177</v>
+      </c>
+      <c r="R217" s="16">
+        <v>40630</v>
+      </c>
+      <c r="S217">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="218" spans="4:19">
+      <c r="D218" t="s">
+        <v>179</v>
+      </c>
+      <c r="E218" s="16">
+        <f t="shared" si="14"/>
+        <v>40630</v>
+      </c>
+      <c r="F218" t="s">
+        <v>50</v>
+      </c>
+      <c r="G218" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.7.3</v>
+      </c>
+      <c r="H218" t="s">
+        <v>49</v>
+      </c>
+      <c r="I218">
+        <f t="shared" si="16"/>
+        <v>201110951</v>
+      </c>
+      <c r="J218" t="s">
+        <v>48</v>
+      </c>
+      <c r="K218">
+        <f t="shared" si="17"/>
+        <v>30</v>
+      </c>
+      <c r="L218" t="s">
+        <v>47</v>
+      </c>
+      <c r="P218">
+        <v>201110951</v>
+      </c>
+      <c r="Q218" t="s">
+        <v>171</v>
+      </c>
+      <c r="R218" s="16">
+        <v>40630</v>
+      </c>
+      <c r="S218">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="219" spans="4:19">
+      <c r="D219" t="s">
+        <v>179</v>
+      </c>
+      <c r="E219" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F219" t="s">
+        <v>50</v>
+      </c>
+      <c r="G219" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.6.1</v>
+      </c>
+      <c r="H219" t="s">
+        <v>49</v>
+      </c>
+      <c r="I219">
+        <f t="shared" si="16"/>
+        <v>201110544</v>
+      </c>
+      <c r="J219" t="s">
+        <v>48</v>
+      </c>
+      <c r="K219">
+        <f t="shared" si="17"/>
+        <v>120</v>
+      </c>
+      <c r="L219" t="s">
+        <v>47</v>
+      </c>
+      <c r="P219">
+        <v>201110544</v>
+      </c>
+      <c r="Q219" t="s">
+        <v>159</v>
+      </c>
+      <c r="R219" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S219">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="220" spans="4:19">
+      <c r="D220" t="s">
+        <v>179</v>
+      </c>
+      <c r="E220" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F220" t="s">
+        <v>50</v>
+      </c>
+      <c r="G220" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.6.2</v>
+      </c>
+      <c r="H220" t="s">
+        <v>49</v>
+      </c>
+      <c r="I220">
+        <f t="shared" si="16"/>
+        <v>201110544</v>
+      </c>
+      <c r="J220" t="s">
+        <v>48</v>
+      </c>
+      <c r="K220">
+        <f t="shared" si="17"/>
+        <v>90</v>
+      </c>
+      <c r="L220" t="s">
+        <v>47</v>
+      </c>
+      <c r="P220">
+        <v>201110544</v>
+      </c>
+      <c r="Q220" t="s">
+        <v>160</v>
+      </c>
+      <c r="R220" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S220">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="221" spans="4:19">
+      <c r="D221" t="s">
+        <v>179</v>
+      </c>
+      <c r="E221" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F221" t="s">
+        <v>50</v>
+      </c>
+      <c r="G221" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.1.1</v>
+      </c>
+      <c r="H221" t="s">
+        <v>49</v>
+      </c>
+      <c r="I221">
+        <f t="shared" si="16"/>
+        <v>201117818</v>
+      </c>
+      <c r="J221" t="s">
+        <v>48</v>
+      </c>
+      <c r="K221">
+        <f t="shared" si="17"/>
+        <v>44</v>
+      </c>
+      <c r="L221" t="s">
+        <v>47</v>
+      </c>
+      <c r="P221">
+        <v>201117818</v>
+      </c>
+      <c r="Q221" t="s">
+        <v>161</v>
+      </c>
+      <c r="R221" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S221">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="222" spans="4:19">
+      <c r="D222" t="s">
+        <v>179</v>
+      </c>
+      <c r="E222" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F222" t="s">
+        <v>50</v>
+      </c>
+      <c r="G222" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.1.3</v>
+      </c>
+      <c r="H222" t="s">
+        <v>49</v>
+      </c>
+      <c r="I222">
+        <f t="shared" si="16"/>
+        <v>201117818</v>
+      </c>
+      <c r="J222" t="s">
+        <v>48</v>
+      </c>
+      <c r="K222">
+        <f t="shared" si="17"/>
+        <v>33</v>
+      </c>
+      <c r="L222" t="s">
+        <v>47</v>
+      </c>
+      <c r="P222">
+        <v>201117818</v>
+      </c>
+      <c r="Q222" t="s">
+        <v>172</v>
+      </c>
+      <c r="R222" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S222">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="223" spans="4:19">
+      <c r="D223" t="s">
+        <v>179</v>
+      </c>
+      <c r="E223" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F223" t="s">
+        <v>50</v>
+      </c>
+      <c r="G223" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.1.4</v>
+      </c>
+      <c r="H223" t="s">
+        <v>49</v>
+      </c>
+      <c r="I223">
+        <f t="shared" si="16"/>
+        <v>201117818</v>
+      </c>
+      <c r="J223" t="s">
+        <v>48</v>
+      </c>
+      <c r="K223">
+        <f t="shared" si="17"/>
+        <v>47</v>
+      </c>
+      <c r="L223" t="s">
+        <v>47</v>
+      </c>
+      <c r="P223">
+        <v>201117818</v>
+      </c>
+      <c r="Q223" t="s">
+        <v>163</v>
+      </c>
+      <c r="R223" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S223">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="224" spans="4:19">
+      <c r="D224" t="s">
+        <v>179</v>
+      </c>
+      <c r="E224" s="16">
+        <f t="shared" si="14"/>
+        <v>40630</v>
+      </c>
+      <c r="F224" t="s">
+        <v>50</v>
+      </c>
+      <c r="G224" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.2.2</v>
+      </c>
+      <c r="H224" t="s">
+        <v>49</v>
+      </c>
+      <c r="I224">
+        <f t="shared" si="16"/>
+        <v>201117818</v>
+      </c>
+      <c r="J224" t="s">
+        <v>48</v>
+      </c>
+      <c r="K224">
+        <f t="shared" si="17"/>
+        <v>64</v>
+      </c>
+      <c r="L224" t="s">
+        <v>47</v>
+      </c>
+      <c r="P224">
+        <v>201117818</v>
+      </c>
+      <c r="Q224" t="s">
+        <v>178</v>
+      </c>
+      <c r="R224" s="16">
+        <v>40630</v>
+      </c>
+      <c r="S224">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="225" spans="4:19">
+      <c r="D225" t="s">
+        <v>179</v>
+      </c>
+      <c r="E225" s="16">
+        <f t="shared" si="14"/>
+        <v>40630</v>
+      </c>
+      <c r="F225" t="s">
+        <v>50</v>
+      </c>
+      <c r="G225" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.2.3</v>
+      </c>
+      <c r="H225" t="s">
+        <v>49</v>
+      </c>
+      <c r="I225">
+        <f t="shared" si="16"/>
+        <v>200819123</v>
+      </c>
+      <c r="J225" t="s">
+        <v>48</v>
+      </c>
+      <c r="K225">
+        <f t="shared" si="17"/>
+        <v>31</v>
+      </c>
+      <c r="L225" t="s">
+        <v>47</v>
+      </c>
+      <c r="P225">
+        <v>200819123</v>
+      </c>
+      <c r="Q225" t="s">
+        <v>164</v>
+      </c>
+      <c r="R225" s="16">
+        <v>40630</v>
+      </c>
+      <c r="S225">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="226" spans="4:19">
+      <c r="D226" t="s">
+        <v>179</v>
+      </c>
+      <c r="E226" s="16">
+        <f t="shared" si="14"/>
+        <v>40630</v>
+      </c>
+      <c r="F226" t="s">
+        <v>50</v>
+      </c>
+      <c r="G226" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.2.3</v>
+      </c>
+      <c r="H226" t="s">
+        <v>49</v>
+      </c>
+      <c r="I226">
+        <f t="shared" si="16"/>
+        <v>201117818</v>
+      </c>
+      <c r="J226" t="s">
+        <v>48</v>
+      </c>
+      <c r="K226">
+        <f t="shared" si="17"/>
+        <v>31</v>
+      </c>
+      <c r="L226" t="s">
+        <v>47</v>
+      </c>
+      <c r="P226">
+        <v>201117818</v>
+      </c>
+      <c r="Q226" t="s">
+        <v>164</v>
+      </c>
+      <c r="R226" s="16">
+        <v>40630</v>
+      </c>
+      <c r="S226">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="227" spans="4:19">
+      <c r="D227" t="s">
+        <v>179</v>
+      </c>
+      <c r="E227" s="16">
+        <f t="shared" si="14"/>
+        <v>40630</v>
+      </c>
+      <c r="F227" t="s">
+        <v>50</v>
+      </c>
+      <c r="G227" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.3.2</v>
+      </c>
+      <c r="H227" t="s">
+        <v>49</v>
+      </c>
+      <c r="I227">
+        <f t="shared" si="16"/>
+        <v>201117818</v>
+      </c>
+      <c r="J227" t="s">
+        <v>48</v>
+      </c>
+      <c r="K227">
+        <f t="shared" si="17"/>
+        <v>26</v>
+      </c>
+      <c r="L227" t="s">
+        <v>47</v>
+      </c>
+      <c r="P227">
+        <v>201117818</v>
+      </c>
+      <c r="Q227" t="s">
+        <v>165</v>
+      </c>
+      <c r="R227" s="16">
+        <v>40630</v>
+      </c>
+      <c r="S227">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="228" spans="4:19">
+      <c r="D228" t="s">
+        <v>179</v>
+      </c>
+      <c r="E228" s="16">
+        <f t="shared" si="14"/>
+        <v>40631</v>
+      </c>
+      <c r="F228" t="s">
+        <v>50</v>
+      </c>
+      <c r="G228" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.6</v>
+      </c>
+      <c r="H228" t="s">
+        <v>49</v>
+      </c>
+      <c r="I228">
+        <f t="shared" si="16"/>
+        <v>201117818</v>
+      </c>
+      <c r="J228" t="s">
+        <v>48</v>
+      </c>
+      <c r="K228">
+        <f t="shared" si="17"/>
+        <v>140</v>
+      </c>
+      <c r="L228" t="s">
+        <v>47</v>
+      </c>
+      <c r="P228">
+        <v>201117818</v>
+      </c>
+      <c r="Q228" t="s">
+        <v>167</v>
+      </c>
+      <c r="R228" s="16">
+        <v>40631</v>
+      </c>
+      <c r="S228">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="229" spans="4:19">
+      <c r="D229" t="s">
+        <v>179</v>
+      </c>
+      <c r="E229" s="16">
+        <f t="shared" si="14"/>
+        <v>40631</v>
+      </c>
+      <c r="F229" t="s">
+        <v>50</v>
+      </c>
+      <c r="G229" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.7</v>
+      </c>
+      <c r="H229" t="s">
+        <v>49</v>
+      </c>
+      <c r="I229">
+        <f t="shared" si="16"/>
+        <v>201117818</v>
+      </c>
+      <c r="J229" t="s">
+        <v>48</v>
+      </c>
+      <c r="K229">
+        <f t="shared" si="17"/>
+        <v>37</v>
+      </c>
+      <c r="L229" t="s">
+        <v>47</v>
+      </c>
+      <c r="P229">
+        <v>201117818</v>
+      </c>
+      <c r="Q229" t="s">
+        <v>168</v>
+      </c>
+      <c r="R229" s="16">
+        <v>40631</v>
+      </c>
+      <c r="S229">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="230" spans="4:19">
+      <c r="D230" t="s">
+        <v>179</v>
+      </c>
+      <c r="E230" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F230" t="s">
+        <v>50</v>
+      </c>
+      <c r="G230" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.6.1</v>
+      </c>
+      <c r="H230" t="s">
+        <v>49</v>
+      </c>
+      <c r="I230">
+        <f t="shared" si="16"/>
+        <v>201117818</v>
+      </c>
+      <c r="J230" t="s">
+        <v>48</v>
+      </c>
+      <c r="K230">
+        <f t="shared" si="17"/>
+        <v>30</v>
+      </c>
+      <c r="L230" t="s">
+        <v>47</v>
+      </c>
+      <c r="P230">
+        <v>201117818</v>
+      </c>
+      <c r="Q230" t="s">
+        <v>159</v>
+      </c>
+      <c r="R230" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S230">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="231" spans="4:19">
+      <c r="D231" t="s">
+        <v>179</v>
+      </c>
+      <c r="E231" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F231" t="s">
+        <v>50</v>
+      </c>
+      <c r="G231" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.6.3</v>
+      </c>
+      <c r="H231" t="s">
+        <v>49</v>
+      </c>
+      <c r="I231">
+        <f t="shared" si="16"/>
+        <v>201117818</v>
+      </c>
+      <c r="J231" t="s">
+        <v>48</v>
+      </c>
+      <c r="K231">
+        <f t="shared" si="17"/>
+        <v>40</v>
+      </c>
+      <c r="L231" t="s">
+        <v>47</v>
+      </c>
+      <c r="P231">
+        <v>201117818</v>
+      </c>
+      <c r="Q231" t="s">
+        <v>176</v>
+      </c>
+      <c r="R231" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S231">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="232" spans="4:19">
+      <c r="D232" t="s">
+        <v>179</v>
+      </c>
+      <c r="E232" s="16">
+        <f t="shared" si="14"/>
+        <v>40632</v>
+      </c>
+      <c r="F232" t="s">
+        <v>50</v>
+      </c>
+      <c r="G232" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.7.1</v>
+      </c>
+      <c r="H232" t="s">
+        <v>49</v>
+      </c>
+      <c r="I232">
+        <f t="shared" si="16"/>
+        <v>201117818</v>
+      </c>
+      <c r="J232" t="s">
+        <v>48</v>
+      </c>
+      <c r="K232">
+        <f t="shared" si="17"/>
+        <v>60</v>
+      </c>
+      <c r="L232" t="s">
+        <v>47</v>
+      </c>
+      <c r="P232">
+        <v>201117818</v>
+      </c>
+      <c r="Q232" t="s">
+        <v>177</v>
+      </c>
+      <c r="R232" s="16">
+        <v>40632</v>
+      </c>
+      <c r="S232">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="233" spans="4:19">
+      <c r="D233" t="s">
+        <v>179</v>
+      </c>
+      <c r="E233" s="16">
+        <f t="shared" si="14"/>
+        <v>40632</v>
+      </c>
+      <c r="F233" t="s">
+        <v>50</v>
+      </c>
+      <c r="G233" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.7.3</v>
+      </c>
+      <c r="H233" t="s">
+        <v>49</v>
+      </c>
+      <c r="I233">
+        <f t="shared" si="16"/>
+        <v>201117818</v>
+      </c>
+      <c r="J233" t="s">
+        <v>48</v>
+      </c>
+      <c r="K233">
+        <f t="shared" si="17"/>
+        <v>34</v>
+      </c>
+      <c r="L233" t="s">
+        <v>47</v>
+      </c>
+      <c r="P233">
+        <v>201117818</v>
+      </c>
+      <c r="Q233" t="s">
+        <v>171</v>
+      </c>
+      <c r="R233" s="16">
+        <v>40632</v>
+      </c>
+      <c r="S233">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="234" spans="4:19">
+      <c r="D234" t="s">
+        <v>179</v>
+      </c>
+      <c r="E234" s="16">
+        <f t="shared" si="14"/>
+        <v>40629</v>
+      </c>
+      <c r="F234" t="s">
+        <v>50</v>
+      </c>
+      <c r="G234" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.6</v>
+      </c>
+      <c r="H234" t="s">
+        <v>49</v>
+      </c>
+      <c r="I234">
+        <f t="shared" si="16"/>
+        <v>200819123</v>
+      </c>
+      <c r="J234" t="s">
+        <v>48</v>
+      </c>
+      <c r="K234">
+        <f t="shared" si="17"/>
+        <v>60</v>
+      </c>
+      <c r="L234" t="s">
+        <v>47</v>
+      </c>
+      <c r="P234">
+        <v>200819123</v>
+      </c>
+      <c r="Q234" t="s">
+        <v>167</v>
+      </c>
+      <c r="R234" s="16">
+        <v>40629</v>
+      </c>
+      <c r="S234">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="235" spans="4:19">
+      <c r="D235" t="s">
+        <v>179</v>
+      </c>
+      <c r="E235" s="16">
+        <f t="shared" si="14"/>
+        <v>40628</v>
+      </c>
+      <c r="F235" t="s">
+        <v>50</v>
+      </c>
+      <c r="G235" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.5.6</v>
+      </c>
+      <c r="H235" t="s">
+        <v>49</v>
+      </c>
+      <c r="I235">
+        <f t="shared" si="16"/>
+        <v>200819123</v>
+      </c>
+      <c r="J235" t="s">
+        <v>48</v>
+      </c>
+      <c r="K235">
+        <f t="shared" si="17"/>
+        <v>60</v>
+      </c>
+      <c r="L235" t="s">
+        <v>47</v>
+      </c>
+      <c r="P235">
+        <v>200819123</v>
+      </c>
+      <c r="Q235" t="s">
+        <v>167</v>
+      </c>
+      <c r="R235" s="16">
+        <v>40628</v>
+      </c>
+      <c r="S235">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="236" spans="4:19">
+      <c r="D236" t="s">
+        <v>179</v>
+      </c>
+      <c r="E236" s="16">
+        <f t="shared" si="14"/>
+        <v>40626</v>
+      </c>
+      <c r="F236" t="s">
+        <v>50</v>
+      </c>
+      <c r="G236" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.2.1</v>
+      </c>
+      <c r="H236" t="s">
+        <v>49</v>
+      </c>
+      <c r="I236">
+        <f t="shared" si="16"/>
+        <v>200819123</v>
+      </c>
+      <c r="J236" t="s">
+        <v>48</v>
+      </c>
+      <c r="K236">
+        <f t="shared" si="17"/>
+        <v>30</v>
+      </c>
+      <c r="L236" t="s">
+        <v>47</v>
+      </c>
+      <c r="P236">
+        <v>200819123</v>
+      </c>
+      <c r="Q236" t="s">
+        <v>173</v>
+      </c>
+      <c r="R236" s="16">
+        <v>40626</v>
+      </c>
+      <c r="S236">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="237" spans="4:19">
+      <c r="D237" t="s">
+        <v>179</v>
+      </c>
+      <c r="E237" s="16">
+        <f t="shared" si="14"/>
+        <v>40626</v>
+      </c>
+      <c r="F237" t="s">
+        <v>50</v>
+      </c>
+      <c r="G237" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.1.3</v>
+      </c>
+      <c r="H237" t="s">
+        <v>49</v>
+      </c>
+      <c r="I237">
+        <f t="shared" si="16"/>
+        <v>200819123</v>
+      </c>
+      <c r="J237" t="s">
+        <v>48</v>
+      </c>
+      <c r="K237">
+        <f t="shared" si="17"/>
+        <v>20</v>
+      </c>
+      <c r="L237" t="s">
+        <v>47</v>
+      </c>
+      <c r="P237">
+        <v>200819123</v>
+      </c>
+      <c r="Q237" t="s">
+        <v>172</v>
+      </c>
+      <c r="R237" s="16">
+        <v>40626</v>
+      </c>
+      <c r="S237">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="238" spans="4:19">
+      <c r="D238" t="s">
+        <v>179</v>
+      </c>
+      <c r="E238" s="16">
+        <f t="shared" si="14"/>
+        <v>40630</v>
+      </c>
+      <c r="F238" t="s">
+        <v>50</v>
+      </c>
+      <c r="G238" t="str">
+        <f t="shared" si="15"/>
+        <v>1.5.7.1</v>
+      </c>
+      <c r="H238" t="s">
+        <v>49</v>
+      </c>
+      <c r="I238">
+        <f t="shared" si="16"/>
+        <v>200819123</v>
+      </c>
+      <c r="J238" t="s">
+        <v>48</v>
+      </c>
+      <c r="K238">
+        <f t="shared" si="17"/>
+        <v>60</v>
+      </c>
+      <c r="L238" t="s">
+        <v>47</v>
+      </c>
+      <c r="P238">
+        <v>200819123</v>
+      </c>
+      <c r="Q238" t="s">
+        <v>177</v>
+      </c>
+      <c r="R238" s="16">
+        <v>40630</v>
+      </c>
+      <c r="S238">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>